<commit_message>
Lấấy số mảnh trích đo 22
</commit_message>
<xml_diff>
--- a/SOMUCKE/TRICHDODIACHINH2024.xlsx
+++ b/SOMUCKE/TRICHDODIACHINH2024.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\SOMUCKE\SOMUCKE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51CBE7C-F9BD-448B-9AB1-4BBE75E7A1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11760" tabRatio="758" activeTab="8"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Khe Sanh" sheetId="3" r:id="rId1"/>
@@ -36,7 +42,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Khe Sanh'!$A$1:$H$1</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -54,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="257">
   <si>
     <t>Mã hồ sơ</t>
   </si>
@@ -819,12 +825,18 @@
   </si>
   <si>
     <t>Đại Độ</t>
+  </si>
+  <si>
+    <t>315/24</t>
+  </si>
+  <si>
+    <t>400+2501.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -1301,14 +1313,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I154"/>
   <sheetViews>
@@ -2283,7 +2295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -2414,7 +2426,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -2466,7 +2478,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -2548,7 +2560,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -2600,7 +2612,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -2652,7 +2664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:H266"/>
   <sheetViews>
@@ -5354,7 +5366,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -5406,7 +5418,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -5458,7 +5470,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -5513,7 +5525,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -5693,7 +5705,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H174"/>
   <sheetViews>
@@ -6936,7 +6948,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:I269"/>
   <sheetViews>
@@ -9939,7 +9951,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:I271"/>
   <sheetViews>
@@ -12963,7 +12975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -12976,7 +12988,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr codeName="Sheet23"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -12989,7 +13001,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -13002,7 +13014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr codeName="Sheet24"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -13015,12 +13027,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5"/>
@@ -13560,6 +13572,32 @@
         <v>988.8</v>
       </c>
     </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="21">
+        <v>22</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="C23" s="21">
+        <v>6</v>
+      </c>
+      <c r="D23" s="21">
+        <v>717</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="21">
+        <v>2901.3</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="H23" s="21" t="s">
+        <v>194</v>
+      </c>
+    </row>
     <row r="39" spans="4:4">
       <c r="D39" s="22"/>
     </row>
@@ -13574,7 +13612,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -13956,7 +13994,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:H42"/>
   <sheetViews>
@@ -14585,7 +14623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -14786,7 +14824,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H23"/>
   <sheetViews>
@@ -15394,7 +15432,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -15662,11 +15700,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
LẤY MẢNH TRÍCH ĐO TÂN LONG 13
</commit_message>
<xml_diff>
--- a/SOMUCKE/TRICHDODIACHINH2024.xlsx
+++ b/SOMUCKE/TRICHDODIACHINH2024.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\SOMUCKE\SOMUCKE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\SOMUCKE\SOMUCKE\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688FF10F-4C5C-49FA-817F-B6B490781F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="758"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Khe Sanh" sheetId="3" r:id="rId1"/>
@@ -41,7 +42,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Khe Sanh'!$A$1:$H$1</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="258">
   <si>
     <t>Mã hồ sơ</t>
   </si>
@@ -830,12 +831,15 @@
   </si>
   <si>
     <t>400+2501.3</t>
+  </si>
+  <si>
+    <t>357/24</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -1319,11 +1323,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
@@ -2317,7 +2321,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -2448,7 +2452,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -2500,7 +2504,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -2582,7 +2586,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -2634,7 +2638,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -2686,7 +2690,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:H266"/>
   <sheetViews>
@@ -5388,7 +5392,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -5440,7 +5444,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -5492,7 +5496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -5547,7 +5551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -5727,7 +5731,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H174"/>
   <sheetViews>
@@ -6970,7 +6974,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:I269"/>
   <sheetViews>
@@ -9973,7 +9977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:I271"/>
   <sheetViews>
@@ -12997,7 +13001,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr codeName="Sheet22"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -13010,7 +13014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr codeName="Sheet23"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -13023,7 +13027,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <sheetPr codeName="Sheet25"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -13036,7 +13040,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr codeName="Sheet24"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -13049,7 +13053,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H46"/>
   <sheetViews>
@@ -13634,7 +13638,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -14016,12 +14020,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14371,12 +14375,27 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="16.5">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
+      <c r="A14" s="21">
+        <v>13</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="C14" s="21">
+        <v>9</v>
+      </c>
+      <c r="D14" s="21">
+        <v>141</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="21">
+        <v>1137.3</v>
+      </c>
+      <c r="G14" s="21">
+        <v>400</v>
+      </c>
       <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8" ht="16.5">
@@ -14645,7 +14664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:H7"/>
   <sheetViews>
@@ -14846,7 +14865,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H23"/>
   <sheetViews>
@@ -15454,7 +15473,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -15722,7 +15741,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:H11"/>
   <sheetViews>

</xml_diff>

<commit_message>
LẤY MẢNH TRÍCH ĐO TÂN LONG 14
</commit_message>
<xml_diff>
--- a/SOMUCKE/TRICHDODIACHINH2024.xlsx
+++ b/SOMUCKE/TRICHDODIACHINH2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\SOMUCKE\SOMUCKE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688FF10F-4C5C-49FA-817F-B6B490781F2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24CB2BD-286E-4066-AAC0-81639F71D0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="259">
   <si>
     <t>Mã hồ sơ</t>
   </si>
@@ -834,6 +834,9 @@
   </si>
   <si>
     <t>357/24</t>
+  </si>
+  <si>
+    <t>358/24</t>
   </si>
 </sst>
 </file>
@@ -14025,7 +14028,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14399,12 +14402,24 @@
       <c r="H14" s="21"/>
     </row>
     <row r="15" spans="1:8" ht="16.5">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
+      <c r="A15" s="21">
+        <v>14</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" s="21">
+        <v>10</v>
+      </c>
+      <c r="D15" s="21">
+        <v>455</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="21">
+        <v>478.6</v>
+      </c>
       <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:8" ht="16.5">

</xml_diff>

<commit_message>
lấy mảnh trích đo tân long số 15
</commit_message>
<xml_diff>
--- a/SOMUCKE/TRICHDODIACHINH2024.xlsx
+++ b/SOMUCKE/TRICHDODIACHINH2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\SOMUCKE\SOMUCKE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24CB2BD-286E-4066-AAC0-81639F71D0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1FB441-986F-417D-B694-2408DD816AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="262">
   <si>
     <t>Mã hồ sơ</t>
   </si>
@@ -837,6 +837,15 @@
   </si>
   <si>
     <t>358/24</t>
+  </si>
+  <si>
+    <t>350/24</t>
+  </si>
+  <si>
+    <t>640;661;654</t>
+  </si>
+  <si>
+    <t>Long Quy</t>
   </si>
 </sst>
 </file>
@@ -14028,7 +14037,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14423,11 +14432,21 @@
       <c r="H15" s="21"/>
     </row>
     <row r="16" spans="1:8" ht="16.5">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
+      <c r="A16" s="21">
+        <v>15</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="C16" s="21">
+        <v>10</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>261</v>
+      </c>
       <c r="F16" s="21"/>
       <c r="H16" s="21"/>
     </row>

</xml_diff>